<commit_message>
add transaction data function update
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stitch.liu\Documents\UiPath\UiPathFramework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workstation\02 coding\RPA\UiPath\StudioProject\Robotic Enterprise Framework(Final)\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BADFFE8-CB52-4F43-88C0-3B70BEB6CC98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F1329B-BF88-4CA1-A1CE-936BACE88C5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -228,6 +228,18 @@
   </si>
   <si>
     <t>Data\Input\SystemAccount.xlsx</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExecutionDataExcelFile</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于启动数据的导入</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data\Input\ExecutionData.xlsx</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -583,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,6 +732,17 @@
       </c>
       <c r="C10" s="7" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>